<commit_message>
pit0 25 micro sec, and motor speed control test
</commit_message>
<xml_diff>
--- a/Pin Guide.xlsx
+++ b/Pin Guide.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Google Drive\workspace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Google Drive\2015 Roboin\SmartCar2015\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23640" windowHeight="7035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23640" windowHeight="7035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="INTURRUPT" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="330">
   <si>
     <t>MPC5606B 방향 외부</t>
   </si>
@@ -1099,6 +1100,10 @@
   </si>
   <si>
     <t>14,15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1548,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1571,6 +1576,9 @@
       <c r="H1" t="s">
         <v>43</v>
       </c>
+      <c r="I1" t="s">
+        <v>329</v>
+      </c>
       <c r="L1" t="s">
         <v>48</v>
       </c>
@@ -1696,6 +1704,9 @@
       <c r="D6" t="s">
         <v>22</v>
       </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
       <c r="H6" t="s">
         <v>52</v>
       </c>
@@ -1710,6 +1721,9 @@
       <c r="D7" t="s">
         <v>23</v>
       </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
       <c r="I7">
         <v>5</v>
       </c>
@@ -1727,6 +1741,9 @@
       <c r="D8" t="s">
         <v>31</v>
       </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
       <c r="I8" s="3">
         <v>6</v>
       </c>
@@ -1743,6 +1760,9 @@
       </c>
       <c r="D9" t="s">
         <v>24</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
       </c>
       <c r="I9" s="3">
         <v>7</v>
@@ -2086,8 +2106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>